<commit_message>
added men and women distribution (separately)
</commit_message>
<xml_diff>
--- a/clear_data/men/men_2015_2022_0.xlsx
+++ b/clear_data/men/men_2015_2022_0.xlsx
@@ -462,7 +462,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>0 - 4 года</t>
+          <t>0 - 4</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -493,7 +493,7 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>5 - 9 лет</t>
+          <t>5 - 9</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -524,7 +524,7 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>10 - 14 лет</t>
+          <t>10 - 14</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -555,7 +555,7 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>15 - 19 лет</t>
+          <t>15 - 19</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -586,7 +586,7 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>20 - 24 лет</t>
+          <t>20 - 24</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -617,7 +617,7 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>25 - 29 лет</t>
+          <t>25 - 29</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -648,7 +648,7 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>30 - 34 лет</t>
+          <t>30 - 34</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -679,7 +679,7 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>35 - 39 лет</t>
+          <t>35 - 39</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -710,7 +710,7 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>40 - 44 лет</t>
+          <t>40 - 44</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -741,7 +741,7 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>45 - 49 лет</t>
+          <t>45 - 49</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -772,7 +772,7 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>50 - 54 лет</t>
+          <t>50 - 54</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -803,7 +803,7 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>55 - 59 лет</t>
+          <t>55 - 59</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -834,7 +834,7 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>60 - 64 лет</t>
+          <t>60 - 64</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -865,7 +865,7 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>65 - 69 лет</t>
+          <t>65 - 69</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -896,7 +896,7 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>70 - 74 лет</t>
+          <t>70 - 74</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -927,7 +927,7 @@
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>75 - 79 лет</t>
+          <t>75 - 79</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -958,7 +958,7 @@
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>80 - 84 лет</t>
+          <t>80 - 84</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -989,7 +989,7 @@
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>85 - 89 лет</t>
+          <t>85 - 89</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -1020,7 +1020,7 @@
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>90 - 94 лет</t>
+          <t>90 - 94</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -1051,7 +1051,7 @@
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>95 - 99 лет</t>
+          <t>95 - 99</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -1082,7 +1082,7 @@
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>100+ лет</t>
+          <t>100+</t>
         </is>
       </c>
       <c r="B22" t="n">

</xml_diff>